<commit_message>
tried something and didnt work so back to what it was
</commit_message>
<xml_diff>
--- a/data/films_messy.xlsx
+++ b/data/films_messy.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mskcc-my.sharepoint.com/personal/kostrzc_mskcc_org/Documents/Biostat Computing/janitor_function_overview/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EB65F835-AA2B-934C-851D-3DC69783D88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:40009_{EB65F835-AA2B-934C-851D-3DC69783D88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BB044D8-E7AB-2E4D-B28A-7A7370FF5832}"/>
   <bookViews>
-    <workbookView xWindow="8440" yWindow="3800" windowWidth="27240" windowHeight="15940"/>
+    <workbookView xWindow="1560" yWindow="2060" windowWidth="27240" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="films_messy" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -987,11 +987,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
should be back to how it was
</commit_message>
<xml_diff>
--- a/data/films_messy.xlsx
+++ b/data/films_messy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mskcc-my.sharepoint.com/personal/kostrzc_mskcc_org/Documents/Biostat Computing/janitor_function_overview/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:40009_{EB65F835-AA2B-934C-851D-3DC69783D88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4BB044D8-E7AB-2E4D-B28A-7A7370FF5832}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:40009_{EB65F835-AA2B-934C-851D-3DC69783D88F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5608E7B5-A7F6-D14B-846E-C625D3977B2F}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="2060" windowWidth="27240" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2320" yWindow="2060" windowWidth="25720" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="films_messy" sheetId="1" r:id="rId1"/>
@@ -689,6 +689,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -991,7 +995,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>